<commit_message>
update template excel, add cancel button login 2fa
</commit_message>
<xml_diff>
--- a/public/exports/sub-constructors.xlsx
+++ b/public/exports/sub-constructors.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>12323</v>
+        <v>123236</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>

</xml_diff>